<commit_message>
CIERRE 14 MAR 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #02  FEBRERO 2022/INVENTARIO ALMACEN  FEBRERO 2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #02  FEBRERO 2022/INVENTARIO ALMACEN  FEBRERO 2022.xlsx
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="68">
   <si>
     <t>INVENTARIO ALMACEN</t>
   </si>
@@ -309,12 +309,6 @@
   </si>
   <si>
     <t># 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO REGISTRA UNA ENTRADA DEL DIA  12 DE FEBRERO </t>
-  </si>
-  <si>
-    <t># 3</t>
   </si>
   <si>
     <t xml:space="preserve">DA SALIDA A UN COMBO POR MENOS ESOS KILOS </t>
@@ -619,7 +613,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -680,12 +674,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="56">
     <border>
@@ -1367,7 +1355,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="252">
+  <cellXfs count="250">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1825,110 +1813,11 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="8" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="33" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="11" fillId="9" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="33" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="33" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1941,9 +1830,6 @@
     </xf>
     <xf numFmtId="2" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1966,6 +1852,102 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="8" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -2286,10 +2268,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="21" x14ac:dyDescent="0.25">
-      <c r="B1" s="201" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="201"/>
+      <c r="B1" s="230" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="230"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -2301,50 +2283,50 @@
       <c r="P1" s="6"/>
     </row>
     <row r="2" spans="2:24" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="202">
+      <c r="B2" s="231">
         <v>44591</v>
       </c>
-      <c r="C2" s="203"/>
-      <c r="F2" s="204" t="s">
+      <c r="C2" s="232"/>
+      <c r="F2" s="233" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="204"/>
-      <c r="H2" s="204"/>
+      <c r="G2" s="233"/>
+      <c r="H2" s="233"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
-      <c r="K2" s="219" t="s">
+      <c r="K2" s="248" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="219"/>
+      <c r="L2" s="248"/>
       <c r="M2" s="8"/>
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11"/>
-      <c r="C3" s="205" t="s">
+      <c r="C3" s="234" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="206"/>
+      <c r="D3" s="235"/>
       <c r="E3" s="11"/>
-      <c r="F3" s="207" t="s">
+      <c r="F3" s="236" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="208"/>
+      <c r="G3" s="237"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="209" t="s">
+      <c r="I3" s="238" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="13"/>
-      <c r="K3" s="219"/>
-      <c r="L3" s="219"/>
-      <c r="M3" s="211" t="s">
+      <c r="K3" s="248"/>
+      <c r="L3" s="248"/>
+      <c r="M3" s="240" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="212"/>
-      <c r="O3" s="213" t="s">
+      <c r="N3" s="241"/>
+      <c r="O3" s="242" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="214"/>
+      <c r="P3" s="243"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
@@ -2366,7 +2348,7 @@
       <c r="H4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="210"/>
+      <c r="I4" s="239"/>
       <c r="J4" s="13"/>
       <c r="K4" s="18" t="s">
         <v>10</v>
@@ -2423,8 +2405,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="215"/>
-      <c r="P5" s="216"/>
+      <c r="O5" s="244"/>
+      <c r="P5" s="245"/>
     </row>
     <row r="6" spans="2:24" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="24" t="s">
@@ -2462,8 +2444,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="217"/>
-      <c r="P6" s="218"/>
+      <c r="O6" s="246"/>
+      <c r="P6" s="247"/>
       <c r="S6" s="37"/>
       <c r="T6" s="38"/>
       <c r="U6" s="39"/>
@@ -2546,8 +2528,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="199"/>
-      <c r="P8" s="200"/>
+      <c r="O8" s="228"/>
+      <c r="P8" s="229"/>
     </row>
     <row r="9" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="24" t="s">
@@ -2628,8 +2610,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="222"/>
-      <c r="P10" s="223"/>
+      <c r="O10" s="220"/>
+      <c r="P10" s="221"/>
       <c r="Q10" s="53"/>
       <c r="R10" s="53"/>
     </row>
@@ -2780,8 +2762,8 @@
         <f>L14+I14</f>
         <v>-34</v>
       </c>
-      <c r="O14" s="224"/>
-      <c r="P14" s="224"/>
+      <c r="O14" s="222"/>
+      <c r="P14" s="222"/>
       <c r="Q14" s="163" t="s">
         <v>47</v>
       </c>
@@ -2995,8 +2977,8 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="O19" s="225"/>
-      <c r="P19" s="225"/>
+      <c r="O19" s="223"/>
+      <c r="P19" s="223"/>
       <c r="Q19" s="163" t="s">
         <v>49</v>
       </c>
@@ -3083,8 +3065,8 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="O21" s="226"/>
-      <c r="P21" s="226"/>
+      <c r="O21" s="224"/>
+      <c r="P21" s="224"/>
       <c r="Q21" s="163" t="s">
         <v>50</v>
       </c>
@@ -3128,8 +3110,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O22" s="227"/>
-      <c r="P22" s="228"/>
+      <c r="O22" s="225"/>
+      <c r="P22" s="226"/>
       <c r="Q22" s="150"/>
       <c r="R22" s="53"/>
       <c r="S22" s="53"/>
@@ -3235,8 +3217,8 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O25" s="229"/>
-      <c r="P25" s="229"/>
+      <c r="O25" s="227"/>
+      <c r="P25" s="227"/>
       <c r="Q25" s="163" t="s">
         <v>51</v>
       </c>
@@ -3628,10 +3610,10 @@
     <row r="37" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="126"/>
       <c r="D37" s="128"/>
-      <c r="F37" s="221" t="s">
+      <c r="F37" s="219" t="s">
         <v>43</v>
       </c>
-      <c r="G37" s="221"/>
+      <c r="G37" s="219"/>
       <c r="H37" s="129">
         <f>SUM(H5:H30)</f>
         <v>35456.6</v>
@@ -3660,7 +3642,7 @@
       <c r="G39" s="1"/>
     </row>
     <row r="40" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B40" s="220" t="s">
+      <c r="B40" s="218" t="s">
         <v>58</v>
       </c>
       <c r="C40" s="155" t="s">
@@ -3681,7 +3663,7 @@
       <c r="N40" s="160"/>
     </row>
     <row r="41" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B41" s="220"/>
+      <c r="B41" s="218"/>
       <c r="C41" s="155" t="s">
         <v>48</v>
       </c>
@@ -3700,7 +3682,7 @@
       <c r="N41" s="160"/>
     </row>
     <row r="42" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B42" s="220"/>
+      <c r="B42" s="218"/>
       <c r="C42" s="155" t="s">
         <v>49</v>
       </c>
@@ -3719,7 +3701,7 @@
       <c r="N42" s="160"/>
     </row>
     <row r="43" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B43" s="220"/>
+      <c r="B43" s="218"/>
       <c r="C43" s="155" t="s">
         <v>50</v>
       </c>
@@ -3738,7 +3720,7 @@
       <c r="N43" s="160"/>
     </row>
     <row r="44" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B44" s="220"/>
+      <c r="B44" s="218"/>
       <c r="C44" s="155" t="s">
         <v>51</v>
       </c>
@@ -3757,7 +3739,7 @@
       <c r="N44" s="160"/>
     </row>
     <row r="45" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B45" s="220"/>
+      <c r="B45" s="218"/>
       <c r="C45" s="155" t="s">
         <v>54</v>
       </c>
@@ -3783,14 +3765,6 @@
     <sortCondition ref="B7:B36"/>
   </sortState>
   <mergeCells count="20">
-    <mergeCell ref="B40:B45"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O25:P25"/>
     <mergeCell ref="O8:P8"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -3803,6 +3777,14 @@
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O6:P6"/>
     <mergeCell ref="K2:L3"/>
+    <mergeCell ref="B40:B45"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O25:P25"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3817,8 +3799,11 @@
   </sheetPr>
   <dimension ref="B1:X45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="Q39" sqref="Q38:Q39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3843,10 +3828,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="21" x14ac:dyDescent="0.25">
-      <c r="B1" s="201" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="201"/>
+      <c r="B1" s="230" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="230"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -3858,50 +3843,50 @@
       <c r="P1" s="6"/>
     </row>
     <row r="2" spans="2:24" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="202">
+      <c r="B2" s="231">
         <v>44619</v>
       </c>
-      <c r="C2" s="203"/>
-      <c r="F2" s="204" t="s">
+      <c r="C2" s="232"/>
+      <c r="F2" s="233" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="204"/>
-      <c r="H2" s="204"/>
+      <c r="G2" s="233"/>
+      <c r="H2" s="233"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
-      <c r="K2" s="219" t="s">
+      <c r="K2" s="248" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="219"/>
+      <c r="L2" s="248"/>
       <c r="M2" s="8"/>
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11"/>
-      <c r="C3" s="205" t="s">
+      <c r="C3" s="234" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="206"/>
+      <c r="D3" s="235"/>
       <c r="E3" s="11"/>
-      <c r="F3" s="207" t="s">
+      <c r="F3" s="236" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="208"/>
+      <c r="G3" s="237"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="209" t="s">
+      <c r="I3" s="238" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="13"/>
-      <c r="K3" s="219"/>
-      <c r="L3" s="219"/>
-      <c r="M3" s="211" t="s">
+      <c r="K3" s="248"/>
+      <c r="L3" s="248"/>
+      <c r="M3" s="240" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="212"/>
-      <c r="O3" s="213" t="s">
+      <c r="N3" s="241"/>
+      <c r="O3" s="242" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="214"/>
+      <c r="P3" s="243"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
@@ -3923,7 +3908,7 @@
       <c r="H4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="210"/>
+      <c r="I4" s="239"/>
       <c r="J4" s="13"/>
       <c r="K4" s="18" t="s">
         <v>10</v>
@@ -3967,21 +3952,21 @@
       </c>
       <c r="J5" s="31"/>
       <c r="K5" s="51">
-        <v>748.87</v>
+        <v>749</v>
       </c>
       <c r="L5" s="52">
         <v>59</v>
       </c>
       <c r="M5" s="32">
         <f>K5-H5</f>
-        <v>0</v>
+        <v>0.12999999999999545</v>
       </c>
       <c r="N5" s="33">
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="215"/>
-      <c r="P5" s="216"/>
+      <c r="O5" s="244"/>
+      <c r="P5" s="245"/>
     </row>
     <row r="6" spans="2:24" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="24" t="s">
@@ -4006,21 +3991,21 @@
       </c>
       <c r="J6" s="31"/>
       <c r="K6" s="51">
-        <v>60.14</v>
+        <v>60.15</v>
       </c>
       <c r="L6" s="52">
         <v>5</v>
       </c>
       <c r="M6" s="35">
         <f t="shared" ref="M6:N21" si="1">K6-H6</f>
-        <v>-1.2000000000000028</v>
+        <v>-1.1900000000000048</v>
       </c>
       <c r="N6" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="217"/>
-      <c r="P6" s="218"/>
+      <c r="O6" s="246"/>
+      <c r="P6" s="247"/>
       <c r="S6" s="37"/>
       <c r="T6" s="38"/>
       <c r="U6" s="39"/>
@@ -4105,8 +4090,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="199"/>
-      <c r="P8" s="199"/>
+      <c r="O8" s="228"/>
+      <c r="P8" s="228"/>
       <c r="Q8" s="193"/>
       <c r="R8" s="1"/>
     </row>
@@ -4178,8 +4163,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="222"/>
-      <c r="P10" s="222"/>
+      <c r="O10" s="220"/>
+      <c r="P10" s="220"/>
       <c r="Q10" s="193"/>
       <c r="R10" s="185"/>
     </row>
@@ -4290,22 +4275,22 @@
       </c>
       <c r="J13" s="31"/>
       <c r="K13" s="51">
-        <v>9126.32</v>
+        <v>9126.4</v>
       </c>
       <c r="L13" s="52">
         <v>295</v>
       </c>
-      <c r="M13" s="231">
+      <c r="M13" s="200">
         <f t="shared" si="1"/>
-        <v>-12.790000000000873</v>
+        <v>-12.710000000000946</v>
       </c>
       <c r="N13" s="192">
         <f t="shared" ref="N13:N33" si="2">L13-I13</f>
         <v>0</v>
       </c>
-      <c r="O13" s="224"/>
-      <c r="P13" s="224"/>
-      <c r="Q13" s="230" t="s">
+      <c r="O13" s="222"/>
+      <c r="P13" s="222"/>
+      <c r="Q13" s="199" t="s">
         <v>64</v>
       </c>
       <c r="R13" s="188"/>
@@ -4425,7 +4410,7 @@
       <c r="S16" s="53"/>
       <c r="T16" s="53"/>
     </row>
-    <row r="17" spans="2:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:20" ht="19.5" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="24" t="s">
         <v>23</v>
       </c>
@@ -4500,14 +4485,14 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O18" s="225"/>
-      <c r="P18" s="225"/>
+      <c r="O18" s="223"/>
+      <c r="P18" s="223"/>
       <c r="Q18" s="187"/>
       <c r="R18" s="185"/>
       <c r="S18" s="53"/>
       <c r="T18" s="53"/>
     </row>
-    <row r="19" spans="2:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:20" ht="19.5" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="72" t="s">
         <v>26</v>
       </c>
@@ -4582,8 +4567,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O20" s="226"/>
-      <c r="P20" s="226"/>
+      <c r="O20" s="224"/>
+      <c r="P20" s="224"/>
       <c r="Q20" s="187"/>
       <c r="R20" s="189"/>
       <c r="S20" s="76"/>
@@ -4596,36 +4581,30 @@
       <c r="C21" s="25"/>
       <c r="D21" s="26"/>
       <c r="E21" s="27"/>
-      <c r="F21" s="25">
-        <v>1404</v>
-      </c>
-      <c r="G21" s="28">
-        <v>108</v>
-      </c>
+      <c r="F21" s="25"/>
+      <c r="G21" s="28"/>
       <c r="H21" s="63">
         <f t="shared" si="0"/>
-        <v>1404</v>
+        <v>0</v>
       </c>
       <c r="I21" s="47">
         <f t="shared" si="0"/>
-        <v>108</v>
+        <v>0</v>
       </c>
       <c r="J21" s="31"/>
       <c r="K21" s="51"/>
       <c r="L21" s="52"/>
       <c r="M21" s="191">
         <f t="shared" si="1"/>
-        <v>-1404</v>
+        <v>0</v>
       </c>
       <c r="N21" s="192">
         <f t="shared" si="2"/>
-        <v>-108</v>
-      </c>
-      <c r="O21" s="227"/>
-      <c r="P21" s="227"/>
-      <c r="Q21" s="232" t="s">
-        <v>66</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="O21" s="225"/>
+      <c r="P21" s="225"/>
+      <c r="Q21" s="187"/>
       <c r="R21" s="185"/>
       <c r="S21" s="53"/>
       <c r="T21" s="53"/>
@@ -4719,21 +4698,21 @@
       </c>
       <c r="J24" s="31"/>
       <c r="K24" s="83">
-        <v>10014.16</v>
+        <v>10014.200000000001</v>
       </c>
       <c r="L24" s="52">
         <v>368</v>
       </c>
       <c r="M24" s="191">
         <f>K24-H24</f>
-        <v>-2.7999999999992724</v>
+        <v>-2.7599999999983993</v>
       </c>
       <c r="N24" s="192">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O24" s="229"/>
-      <c r="P24" s="229"/>
+      <c r="O24" s="227"/>
+      <c r="P24" s="227"/>
       <c r="Q24" s="187"/>
       <c r="R24" s="1"/>
     </row>
@@ -4827,7 +4806,7 @@
       <c r="J27" s="31"/>
       <c r="K27" s="83"/>
       <c r="L27" s="52"/>
-      <c r="M27" s="236">
+      <c r="M27" s="203">
         <f t="shared" si="3"/>
         <v>-24</v>
       </c>
@@ -4837,8 +4816,8 @@
       </c>
       <c r="O27" s="91"/>
       <c r="P27" s="179"/>
-      <c r="Q27" s="235" t="s">
-        <v>68</v>
+      <c r="Q27" s="202" t="s">
+        <v>66</v>
       </c>
       <c r="R27" s="185"/>
       <c r="S27" s="53"/>
@@ -5047,14 +5026,14 @@
       </c>
       <c r="J33" s="31"/>
       <c r="K33" s="83">
-        <v>371.94</v>
+        <v>372</v>
       </c>
       <c r="L33" s="52">
         <v>30</v>
       </c>
       <c r="M33" s="191">
         <f t="shared" si="3"/>
-        <v>-2.9700000000000273</v>
+        <v>-2.910000000000025</v>
       </c>
       <c r="N33" s="192">
         <f t="shared" si="2"/>
@@ -5134,22 +5113,22 @@
     <row r="36" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="126"/>
       <c r="D36" s="128"/>
-      <c r="F36" s="221" t="s">
+      <c r="F36" s="219" t="s">
         <v>43</v>
       </c>
-      <c r="G36" s="221"/>
+      <c r="G36" s="219"/>
       <c r="H36" s="129">
         <f>SUM(H5:H29)</f>
-        <v>23468.760000000002</v>
+        <v>22064.760000000002</v>
       </c>
       <c r="I36" s="130">
         <f>SUM(I5:I29)</f>
-        <v>966</v>
+        <v>858</v>
       </c>
       <c r="J36" s="131"/>
       <c r="K36" s="132">
         <f>SUM(K5:K34)</f>
-        <v>22638.62</v>
+        <v>22638.940000000002</v>
       </c>
       <c r="L36" s="133" t="s">
         <v>63</v>
@@ -5175,68 +5154,64 @@
       <c r="G38" s="1"/>
     </row>
     <row r="39" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="220" t="s">
+      <c r="B39" s="218" t="s">
         <v>58</v>
       </c>
       <c r="C39" s="155" t="s">
         <v>47</v>
       </c>
-      <c r="D39" s="247" t="s">
+      <c r="D39" s="213" t="s">
         <v>65</v>
       </c>
-      <c r="E39" s="248"/>
-      <c r="F39" s="248"/>
-      <c r="G39" s="249"/>
-      <c r="H39" s="249"/>
-      <c r="I39" s="249"/>
-      <c r="J39" s="249"/>
-      <c r="K39" s="249"/>
-      <c r="L39" s="250"/>
-      <c r="M39" s="245"/>
-      <c r="N39" s="246"/>
+      <c r="E39" s="214"/>
+      <c r="F39" s="214"/>
+      <c r="G39" s="215"/>
+      <c r="H39" s="215"/>
+      <c r="I39" s="215"/>
+      <c r="J39" s="215"/>
+      <c r="K39" s="215"/>
+      <c r="L39" s="216"/>
+      <c r="M39" s="211"/>
+      <c r="N39" s="212"/>
     </row>
     <row r="40" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="220"/>
-      <c r="C40" s="233" t="s">
+      <c r="B40" s="218"/>
+      <c r="C40" s="204"/>
+      <c r="D40" s="213"/>
+      <c r="E40" s="214"/>
+      <c r="F40" s="214"/>
+      <c r="G40" s="215"/>
+      <c r="H40" s="215"/>
+      <c r="I40" s="215"/>
+      <c r="J40" s="215"/>
+      <c r="K40" s="215"/>
+      <c r="L40" s="216"/>
+      <c r="M40" s="211"/>
+      <c r="N40" s="212"/>
+    </row>
+    <row r="41" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="218"/>
+      <c r="C41" s="201" t="s">
         <v>48</v>
       </c>
-      <c r="D40" s="247" t="s">
+      <c r="D41" s="217" t="s">
         <v>67</v>
       </c>
-      <c r="E40" s="248"/>
-      <c r="F40" s="248"/>
-      <c r="G40" s="249"/>
-      <c r="H40" s="249"/>
-      <c r="I40" s="249"/>
-      <c r="J40" s="249"/>
-      <c r="K40" s="249"/>
-      <c r="L40" s="250"/>
-      <c r="M40" s="245"/>
-      <c r="N40" s="246"/>
-    </row>
-    <row r="41" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="220"/>
-      <c r="C41" s="234" t="s">
-        <v>49</v>
-      </c>
-      <c r="D41" s="251" t="s">
-        <v>69</v>
-      </c>
-      <c r="E41" s="249"/>
-      <c r="F41" s="249"/>
-      <c r="G41" s="249"/>
-      <c r="H41" s="249"/>
-      <c r="I41" s="249"/>
-      <c r="J41" s="249"/>
-      <c r="K41" s="249"/>
-      <c r="L41" s="250"/>
-      <c r="M41" s="245"/>
-      <c r="N41" s="246"/>
+      <c r="E41" s="215"/>
+      <c r="F41" s="215"/>
+      <c r="G41" s="215"/>
+      <c r="H41" s="215"/>
+      <c r="I41" s="215"/>
+      <c r="J41" s="215"/>
+      <c r="K41" s="215"/>
+      <c r="L41" s="216"/>
+      <c r="M41" s="211"/>
+      <c r="N41" s="212"/>
     </row>
     <row r="42" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B42" s="238"/>
-      <c r="C42" s="237"/>
-      <c r="D42" s="239"/>
+      <c r="B42" s="249"/>
+      <c r="C42" s="204"/>
+      <c r="D42" s="205"/>
       <c r="E42" s="185"/>
       <c r="F42" s="185"/>
       <c r="G42" s="185"/>
@@ -5244,14 +5219,14 @@
       <c r="I42" s="185"/>
       <c r="J42" s="185"/>
       <c r="K42" s="185"/>
-      <c r="L42" s="240"/>
-      <c r="M42" s="241"/>
-      <c r="N42" s="242"/>
+      <c r="L42" s="206"/>
+      <c r="M42" s="207"/>
+      <c r="N42" s="208"/>
     </row>
     <row r="43" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B43" s="238"/>
-      <c r="C43" s="237"/>
-      <c r="D43" s="243"/>
+      <c r="B43" s="249"/>
+      <c r="C43" s="204"/>
+      <c r="D43" s="209"/>
       <c r="E43" s="185"/>
       <c r="F43" s="185"/>
       <c r="G43" s="185"/>
@@ -5259,14 +5234,14 @@
       <c r="I43" s="185"/>
       <c r="J43" s="185"/>
       <c r="K43" s="185"/>
-      <c r="L43" s="240"/>
-      <c r="M43" s="241"/>
-      <c r="N43" s="242"/>
+      <c r="L43" s="206"/>
+      <c r="M43" s="207"/>
+      <c r="N43" s="208"/>
     </row>
     <row r="44" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B44" s="238"/>
-      <c r="C44" s="237"/>
-      <c r="D44" s="244"/>
+      <c r="B44" s="249"/>
+      <c r="C44" s="204"/>
+      <c r="D44" s="210"/>
       <c r="E44" s="185"/>
       <c r="F44" s="185"/>
       <c r="G44" s="185"/>
@@ -5274,9 +5249,9 @@
       <c r="I44" s="185"/>
       <c r="J44" s="185"/>
       <c r="K44" s="185"/>
-      <c r="L44" s="240"/>
-      <c r="M44" s="241"/>
-      <c r="N44" s="242"/>
+      <c r="L44" s="206"/>
+      <c r="M44" s="207"/>
+      <c r="N44" s="208"/>
     </row>
     <row r="45" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C45" s="149"/>
@@ -5286,18 +5261,6 @@
     <sortCondition ref="B9:B16"/>
   </sortState>
   <mergeCells count="20">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="K2:L3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O8:P8"/>
     <mergeCell ref="O24:P24"/>
     <mergeCell ref="F36:G36"/>
     <mergeCell ref="B39:B44"/>
@@ -5306,6 +5269,18 @@
     <mergeCell ref="O18:P18"/>
     <mergeCell ref="O20:P20"/>
     <mergeCell ref="O21:P21"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="K2:L3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:I4"/>
   </mergeCells>
   <pageMargins left="0.27559055118110237" right="0.27559055118110237" top="0.35433070866141736" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="85" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>